<commit_message>
Adicionados os arquivos de entrada e saída da simulação e os arquivos de treinamento da falha 'FSeDG'. Faltando realizar a validação.
</commit_message>
<xml_diff>
--- a/planilhas/outras/falhas.xlsx
+++ b/planilhas/outras/falhas.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Falhas a serem testadas" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="72">
   <si>
     <t>Grupo</t>
   </si>
@@ -151,9 +151,6 @@
     <t>Até -3 Volts</t>
   </si>
   <si>
-    <t>Até ± 1 Volt</t>
-  </si>
-  <si>
     <t>FADG</t>
   </si>
   <si>
@@ -267,12 +264,18 @@
   <si>
     <t>[20 21]</t>
   </si>
+  <si>
+    <t>Até -1 Volt</t>
+  </si>
+  <si>
+    <t>[Vazamento] Considera-se que a água que vaza do tanque 1 não entra no tanque inferior e a água que vaza do tanque 2 retorna ao reservatório.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -391,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -404,15 +407,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -472,6 +466,18 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -562,7 +568,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -597,7 +602,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Escritório">
@@ -773,14 +777,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:K24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:K34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="B27" sqref="B27:K27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.5703125" customWidth="1"/>
     <col min="3" max="3" width="16.140625" bestFit="1" customWidth="1"/>
@@ -793,14 +797,14 @@
     <col min="11" max="11" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
+    <row r="2" spans="2:11">
+      <c r="B2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="C2" s="27"/>
+      <c r="D2" s="28"/>
+    </row>
+    <row r="3" spans="2:11">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -811,7 +815,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:11">
       <c r="B4" s="1">
         <v>0</v>
       </c>
@@ -822,7 +826,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:11">
       <c r="B5" s="1">
         <v>1</v>
       </c>
@@ -833,7 +837,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11">
       <c r="B6" s="1">
         <v>2</v>
       </c>
@@ -844,7 +848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:11">
       <c r="B7" s="1">
         <v>3</v>
       </c>
@@ -855,10 +859,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:11">
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:11">
       <c r="B9" s="2" t="s">
         <v>12</v>
       </c>
@@ -868,16 +872,16 @@
       <c r="D9" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="11" t="s">
         <v>15</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="11" t="s">
+      <c r="G9" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>28</v>
       </c>
       <c r="I9" s="5" t="s">
@@ -890,7 +894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:11">
       <c r="B10" s="1">
         <v>1</v>
       </c>
@@ -900,29 +904,29 @@
       <c r="D10" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="H10" s="9" t="s">
+      <c r="G10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="17">
+      <c r="I10" s="14">
         <v>0.8</v>
       </c>
-      <c r="J10" s="17">
+      <c r="J10" s="14">
         <v>1.2</v>
       </c>
-      <c r="K10" s="26" t="s">
+      <c r="K10" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11">
       <c r="B11" s="1">
         <v>1</v>
       </c>
@@ -932,29 +936,29 @@
       <c r="D11" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="6" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="H11" s="21">
-        <v>1</v>
-      </c>
-      <c r="I11" s="17">
+      <c r="G11" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H11" s="18">
+        <v>1</v>
+      </c>
+      <c r="I11" s="14">
         <v>-3</v>
       </c>
-      <c r="J11" s="17">
+      <c r="J11" s="14">
         <v>3</v>
       </c>
-      <c r="K11" s="26" t="s">
+      <c r="K11" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11">
       <c r="B12" s="1">
         <v>1</v>
       </c>
@@ -964,73 +968,73 @@
       <c r="D12" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
       <c r="F12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G12" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="H12" s="21">
-        <v>1</v>
-      </c>
-      <c r="I12" s="17">
+      <c r="G12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H12" s="18">
+        <v>1</v>
+      </c>
+      <c r="I12" s="14">
         <v>0</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="14">
         <v>0.03</v>
       </c>
-      <c r="K12" s="26" t="s">
+      <c r="K12" s="23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="2:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" s="13" customFormat="1">
       <c r="B13" s="1">
         <v>1</v>
       </c>
-      <c r="C13" s="12">
+      <c r="C13" s="9">
         <v>3</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="9" t="s">
+      <c r="E13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="12" t="s">
+      <c r="F13" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G13" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="H13" s="9" t="s">
+      <c r="G13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="I13" s="18">
+      <c r="I13" s="15">
         <v>0</v>
       </c>
-      <c r="J13" s="18">
+      <c r="J13" s="15">
         <v>0</v>
       </c>
-      <c r="K13" s="26" t="s">
+      <c r="K13" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:11" s="16" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
-      <c r="F14" s="10"/>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="20"/>
-    </row>
-    <row r="15" spans="2:11" s="16" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" s="13" customFormat="1" ht="3.75" customHeight="1">
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="17"/>
+    </row>
+    <row r="15" spans="2:11" s="13" customFormat="1">
       <c r="B15" s="1">
         <v>2</v>
       </c>
@@ -1040,29 +1044,29 @@
       <c r="D15" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="E15" s="9" t="s">
+      <c r="E15" s="6" t="s">
         <v>19</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H15" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I15" s="17">
+      <c r="I15" s="14">
         <v>0.8</v>
       </c>
-      <c r="J15" s="17">
-        <v>1</v>
-      </c>
-      <c r="K15" s="26" t="s">
+      <c r="J15" s="14">
+        <v>1</v>
+      </c>
+      <c r="K15" s="23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11">
       <c r="B16" s="4">
         <v>2</v>
       </c>
@@ -1072,29 +1076,29 @@
       <c r="D16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="25" t="s">
+      <c r="E16" s="22" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G16" s="25" t="s">
-        <v>56</v>
-      </c>
-      <c r="H16" s="22">
-        <v>1</v>
-      </c>
-      <c r="I16" s="23">
+        <v>39</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="H16" s="19">
+        <v>1</v>
+      </c>
+      <c r="I16" s="20">
         <v>-1</v>
       </c>
-      <c r="J16" s="23">
-        <v>1</v>
-      </c>
-      <c r="K16" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="J16" s="20">
+        <v>0</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11">
       <c r="B17" s="1">
         <v>2</v>
       </c>
@@ -1104,29 +1108,29 @@
       <c r="D17" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="E17" s="9" t="s">
+      <c r="E17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="H17" s="21">
-        <v>1</v>
-      </c>
-      <c r="I17" s="17">
+        <v>40</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="H17" s="18">
+        <v>1</v>
+      </c>
+      <c r="I17" s="14">
         <v>0</v>
       </c>
-      <c r="J17" s="17">
+      <c r="J17" s="14">
         <v>0.03</v>
       </c>
-      <c r="K17" s="26" t="s">
+      <c r="K17" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11">
       <c r="B18" s="1">
         <v>2</v>
       </c>
@@ -1134,31 +1138,31 @@
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="E18" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="1" t="s">
+      <c r="G18" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="I18" s="17">
-        <v>0.8</v>
-      </c>
-      <c r="J18" s="17">
-        <v>1.5</v>
-      </c>
-      <c r="K18" s="26" t="s">
+      <c r="I18" s="14">
+        <v>0.7</v>
+      </c>
+      <c r="J18" s="14">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="K18" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:11">
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -1168,41 +1172,41 @@
       <c r="D19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="9" t="s">
+      <c r="E19" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="H19" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="I19" s="17">
+      <c r="I19" s="14">
         <v>0</v>
       </c>
-      <c r="J19" s="17">
+      <c r="J19" s="14">
         <v>0</v>
       </c>
-      <c r="K19" s="26" t="s">
+      <c r="K19" s="23" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="2:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
-      <c r="I20" s="24"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="27"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:11" ht="3.75" customHeight="1">
+      <c r="B20" s="10"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="10"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="10"/>
+      <c r="G20" s="10"/>
+      <c r="H20" s="10"/>
+      <c r="I20" s="21"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="24"/>
+    </row>
+    <row r="21" spans="2:11">
       <c r="B21" s="1">
         <v>3</v>
       </c>
@@ -1210,31 +1214,31 @@
         <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="F21" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" s="17">
+      <c r="G21" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I21" s="14">
         <v>0.25</v>
       </c>
-      <c r="J21" s="17">
+      <c r="J21" s="14">
         <v>0.75</v>
       </c>
-      <c r="K21" s="26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K21" s="23" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11">
       <c r="B22" s="1">
         <v>3</v>
       </c>
@@ -1242,31 +1246,31 @@
         <v>2</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E22" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="G22" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H22" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I22" s="17">
+      <c r="H22" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I22" s="14">
         <v>0.75</v>
       </c>
-      <c r="J22" s="17">
+      <c r="J22" s="14">
         <v>1.25</v>
       </c>
-      <c r="K22" s="28" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="K22" s="25" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11">
       <c r="B23" s="1">
         <v>3</v>
       </c>
@@ -1274,31 +1278,31 @@
         <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="E23" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F23" s="1" t="s">
+      <c r="G23" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H23" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I23" s="17">
+      <c r="I23" s="14">
         <v>0.8</v>
       </c>
-      <c r="J23" s="17">
-        <v>1</v>
-      </c>
-      <c r="K23" s="26" t="s">
+      <c r="J23" s="14">
+        <v>1</v>
+      </c>
+      <c r="K23" s="23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:11">
       <c r="B24" s="1">
         <v>3</v>
       </c>
@@ -1306,35 +1310,154 @@
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="E24" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G24" s="9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H24" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I24" s="17">
+      <c r="G24" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="I24" s="14">
         <v>0</v>
       </c>
-      <c r="J24" s="17">
-        <v>0</v>
-      </c>
-      <c r="K24" s="26" t="s">
+      <c r="J24" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="K24" s="23" t="s">
         <v>11</v>
       </c>
     </row>
+    <row r="26" spans="2:11">
+      <c r="B26" s="29" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+    </row>
+    <row r="27" spans="2:11">
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+    </row>
+    <row r="28" spans="2:11">
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
+    </row>
+    <row r="29" spans="2:11">
+      <c r="B29" s="29"/>
+      <c r="C29" s="29"/>
+      <c r="D29" s="29"/>
+      <c r="E29" s="29"/>
+      <c r="F29" s="29"/>
+      <c r="G29" s="29"/>
+      <c r="H29" s="29"/>
+      <c r="I29" s="29"/>
+      <c r="J29" s="29"/>
+      <c r="K29" s="29"/>
+    </row>
+    <row r="30" spans="2:11">
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="29"/>
+      <c r="G30" s="29"/>
+      <c r="H30" s="29"/>
+      <c r="I30" s="29"/>
+      <c r="J30" s="29"/>
+      <c r="K30" s="29"/>
+    </row>
+    <row r="31" spans="2:11">
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="29"/>
+      <c r="E31" s="29"/>
+      <c r="F31" s="29"/>
+      <c r="G31" s="29"/>
+      <c r="H31" s="29"/>
+      <c r="I31" s="29"/>
+      <c r="J31" s="29"/>
+      <c r="K31" s="29"/>
+    </row>
+    <row r="32" spans="2:11">
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="29"/>
+      <c r="G32" s="29"/>
+      <c r="H32" s="29"/>
+      <c r="I32" s="29"/>
+      <c r="J32" s="29"/>
+      <c r="K32" s="29"/>
+    </row>
+    <row r="33" spans="2:11">
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="29"/>
+      <c r="H33" s="29"/>
+      <c r="I33" s="29"/>
+      <c r="J33" s="29"/>
+      <c r="K33" s="29"/>
+    </row>
+    <row r="34" spans="2:11">
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="29"/>
+      <c r="E34" s="29"/>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="29"/>
+      <c r="I34" s="29"/>
+      <c r="J34" s="29"/>
+      <c r="K34" s="29"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="10">
+    <mergeCell ref="B30:K30"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="B32:K32"/>
+    <mergeCell ref="B33:K33"/>
+    <mergeCell ref="B34:K34"/>
     <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B26:K26"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="B28:K28"/>
+    <mergeCell ref="B29:K29"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>